<commit_message>
updates from personal laptop Friday night
</commit_message>
<xml_diff>
--- a/Tables/Formatted/Segment Pivot.xlsx
+++ b/Tables/Formatted/Segment Pivot.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gorbetw\Documents\Repos\AI-Detection\Tables\Formatted\"/>
@@ -14,15 +14,12 @@
   <sheets>
     <sheet name="segment-pivot" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Segment</t>
-  </si>
   <si>
     <t>Greater than 90% chance of being AI generated</t>
   </si>
@@ -39,13 +36,16 @@
     <t>Greater than 50% chance of being AI generated</t>
   </si>
   <si>
-    <t>Less than 50% chance of being AI generated</t>
+    <t>Greater than 50% chance of being real</t>
+  </si>
+  <si>
+    <t>Percentage of abstract words</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -197,7 +197,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="40">
+  <fills count="46">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -419,8 +419,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7E2F5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFDAB9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC3EFC3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5C7C7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDBCDE9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -546,8 +582,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -590,8 +668,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -638,14 +717,92 @@
     <xf numFmtId="0" fontId="13" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="38" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="39" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="19" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="19" fillId="39" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="40" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="40" borderId="10" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="40" borderId="13" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="41" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="41" borderId="10" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="41" borderId="13" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="42" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="42" borderId="10" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="42" borderId="13" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="43" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="43" borderId="10" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="43" borderId="13" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="44" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="44" borderId="10" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="44" borderId="13" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="45" borderId="11" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="45" borderId="12" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="45" borderId="14" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -685,193 +842,25 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="42" builtinId="5"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2" tint="-0.749992370372631"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFA3D0EF"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFD8C7E7"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFF0AAAA"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF9FE59F"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFC693"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thick">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom style="thick">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFF2F2F2"/>
+      <color rgb="FFDBCDE9"/>
+      <color rgb="FFF5C7C7"/>
+      <color rgb="FFC3EFC3"/>
+      <color rgb="FFFFDAB9"/>
+      <color rgb="FFC7E2F5"/>
       <color rgb="FFD8C7E7"/>
       <color rgb="FFF0AAAA"/>
       <color rgb="FF9FE59F"/>
       <color rgb="FFA3D0EF"/>
-      <color rgb="FFFFC693"/>
     </mruColors>
   </colors>
   <extLst>
@@ -883,21 +872,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:H5" totalsRowShown="0" headerRowDxfId="7" dataDxfId="9" tableBorderDxfId="8">
-  <tableColumns count="7">
-    <tableColumn id="1" name="Segment" dataDxfId="0"/>
-    <tableColumn id="2" name="Greater than 90% chance of being AI generated" dataDxfId="1"/>
-    <tableColumn id="3" name="Greater than 80% chance of being AI generated" dataDxfId="6"/>
-    <tableColumn id="4" name="Greater than 70% chance of being AI generated" dataDxfId="5"/>
-    <tableColumn id="5" name="Greater than 60% chance of being AI generated" dataDxfId="4"/>
-    <tableColumn id="6" name="Greater than 50% chance of being AI generated" dataDxfId="3"/>
-    <tableColumn id="7" name="Less than 50% chance of being AI generated" dataDxfId="2"/>
-  </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1163,117 +1137,183 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H5"/>
+  <dimension ref="B2:N6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="11" style="1" customWidth="1"/>
-    <col min="3" max="8" width="13.7109375" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="14" width="13.7109375" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="D2" s="22"/>
+      <c r="E2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="F2" s="22"/>
+      <c r="G2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="H2" s="22"/>
+      <c r="I2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="J2" s="22"/>
+      <c r="K2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="L2" s="22"/>
+      <c r="M2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="17" t="s">
-        <v>6</v>
-      </c>
+      <c r="N2" s="23"/>
     </row>
-    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="16">
+    <row r="3" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="24">
         <v>0.25</v>
       </c>
       <c r="C3" s="5">
         <v>779</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="26">
+        <v>5.39997227228615E-2</v>
+      </c>
+      <c r="E3" s="3">
         <v>426</v>
       </c>
-      <c r="E3" s="7">
+      <c r="F3" s="29">
+        <v>2.9530015250242618E-2</v>
+      </c>
+      <c r="G3" s="7">
         <v>356</v>
       </c>
-      <c r="F3" s="9">
+      <c r="H3" s="32">
+        <v>2.467766532649383E-2</v>
+      </c>
+      <c r="I3" s="9">
         <v>339</v>
       </c>
-      <c r="G3" s="11">
+      <c r="J3" s="35">
+        <v>2.3499237487869126E-2</v>
+      </c>
+      <c r="K3" s="11">
         <v>390</v>
       </c>
-      <c r="H3" s="13">
+      <c r="L3" s="38">
+        <v>2.7034521003743241E-2</v>
+      </c>
+      <c r="M3" s="13">
         <v>12136</v>
       </c>
+      <c r="N3" s="41">
+        <v>0.84125883820878966</v>
+      </c>
     </row>
-    <row r="4" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="16">
+    <row r="4" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="24">
         <v>0.5</v>
       </c>
       <c r="C4" s="6">
         <v>680</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="27">
+        <v>4.7137113544988216E-2</v>
+      </c>
+      <c r="E4" s="4">
         <v>220</v>
       </c>
-      <c r="E4" s="8">
+      <c r="F4" s="30">
+        <v>1.5250242617496187E-2</v>
+      </c>
+      <c r="G4" s="8">
         <v>165</v>
       </c>
-      <c r="F4" s="10">
+      <c r="H4" s="33">
+        <v>1.1437681963122141E-2</v>
+      </c>
+      <c r="I4" s="10">
         <v>165</v>
       </c>
-      <c r="G4" s="12">
+      <c r="J4" s="36">
+        <v>1.1437681963122141E-2</v>
+      </c>
+      <c r="K4" s="12">
         <v>168</v>
       </c>
-      <c r="H4" s="14">
+      <c r="L4" s="39">
+        <v>1.1645639816997089E-2</v>
+      </c>
+      <c r="M4" s="14">
         <v>13028</v>
       </c>
+      <c r="N4" s="42">
+        <v>0.90309164009427423</v>
+      </c>
     </row>
-    <row r="5" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="16">
+    <row r="5" spans="2:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="25">
         <v>1</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="16">
         <v>507</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="28">
+        <v>3.5144877304866214E-2</v>
+      </c>
+      <c r="E5" s="17">
         <v>120</v>
       </c>
-      <c r="E5" s="7">
+      <c r="F5" s="31">
+        <v>8.318314154997921E-3</v>
+      </c>
+      <c r="G5" s="18">
         <v>77</v>
       </c>
-      <c r="F5" s="9">
+      <c r="H5" s="34">
+        <v>5.3375849161236659E-3</v>
+      </c>
+      <c r="I5" s="19">
         <v>84</v>
       </c>
-      <c r="G5" s="11">
+      <c r="J5" s="37">
+        <v>5.8228199084985445E-3</v>
+      </c>
+      <c r="K5" s="20">
         <v>80</v>
       </c>
-      <c r="H5" s="13">
+      <c r="L5" s="40">
+        <v>5.545542769998614E-3</v>
+      </c>
+      <c r="M5" s="21">
         <v>13558</v>
       </c>
+      <c r="N5" s="43">
+        <v>0.93983086094551505</v>
+      </c>
     </row>
+    <row r="6" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>